<commit_message>
added validation to ensure at least one criterion is selected per category; prepared for hydrogen datasets
</commit_message>
<xml_diff>
--- a/combined_wide_CLEAN.xlsx
+++ b/combined_wide_CLEAN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P246"/>
+  <dimension ref="A1:Q246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,11 @@
       <c r="P1" s="1" t="inlineStr">
         <is>
           <t>trade freedom</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>renewable energy readiness</t>
         </is>
       </c>
     </row>
@@ -540,6 +545,7 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -566,6 +572,7 @@
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -604,6 +611,9 @@
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="n">
+        <v>0.1047945415047578</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -630,6 +640,7 @@
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -678,6 +689,9 @@
       <c r="P6" t="n">
         <v>0.4999999999999999</v>
       </c>
+      <c r="Q6" t="n">
+        <v>0.2914971085885629</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -725,6 +739,9 @@
       </c>
       <c r="P7" t="n">
         <v>0.765151515151515</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.5546308478413855</v>
       </c>
     </row>
     <row r="8">
@@ -752,6 +769,7 @@
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -778,6 +796,7 @@
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -828,6 +847,9 @@
       <c r="P10" t="n">
         <v>0.678030303030303</v>
       </c>
+      <c r="Q10" t="n">
+        <v>0.58792032555151</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -878,6 +900,9 @@
       <c r="P11" t="n">
         <v>0.3106060606060606</v>
       </c>
+      <c r="Q11" t="n">
+        <v>0.5385674509683934</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -929,6 +954,9 @@
       </c>
       <c r="P12" t="n">
         <v>0.5946969696969696</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.3841140654162715</v>
       </c>
     </row>
     <row r="13">
@@ -962,6 +990,7 @@
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1014,6 +1043,9 @@
       <c r="P14" t="n">
         <v>0.9015151515151515</v>
       </c>
+      <c r="Q14" t="n">
+        <v>0.7509102591561364</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1065,6 +1097,9 @@
       </c>
       <c r="P15" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.9179695866352537</v>
       </c>
     </row>
     <row r="16">
@@ -1112,6 +1147,9 @@
       <c r="P16" t="n">
         <v>0.5075757575757576</v>
       </c>
+      <c r="Q16" t="n">
+        <v>0.09515650338096258</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1160,6 +1198,9 @@
       <c r="P17" t="n">
         <v>0.1401515151515151</v>
       </c>
+      <c r="Q17" t="n">
+        <v>0.08597741945353855</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1211,6 +1252,9 @@
       </c>
       <c r="P18" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.8967659027629041</v>
       </c>
     </row>
     <row r="19">
@@ -1260,6 +1304,9 @@
       <c r="P19" t="n">
         <v>0.356060606060606</v>
       </c>
+      <c r="Q19" t="n">
+        <v>0.1418168466787015</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1308,6 +1355,9 @@
       <c r="P20" t="n">
         <v>0.3484848484848485</v>
       </c>
+      <c r="Q20" t="n">
+        <v>0.2625829942171771</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1358,6 +1408,9 @@
       <c r="P21" t="n">
         <v>0.3749999999999999</v>
       </c>
+      <c r="Q21" t="n">
+        <v>0.2744546094299789</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1408,6 +1461,9 @@
       <c r="P22" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q22" t="n">
+        <v>0.7172842150353395</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1456,6 +1512,9 @@
       <c r="P23" t="n">
         <v>0.8143939393939394</v>
       </c>
+      <c r="Q23" t="n">
+        <v>0.1499250374812594</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1504,6 +1563,7 @@
       <c r="P24" t="n">
         <v>0.1401515151515151</v>
       </c>
+      <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1550,6 +1610,9 @@
       <c r="P25" t="n">
         <v>0.4886363636363636</v>
       </c>
+      <c r="Q25" t="n">
+        <v>0.379096166202613</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1599,6 +1662,9 @@
       </c>
       <c r="P26" t="n">
         <v>0.5416666666666666</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.2245815867576415</v>
       </c>
     </row>
     <row r="27">
@@ -1646,6 +1712,7 @@
       <c r="P27" t="n">
         <v>0.2462121212121212</v>
       </c>
+      <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1698,6 +1765,9 @@
       <c r="P28" t="n">
         <v>0.3484848484848485</v>
       </c>
+      <c r="Q28" t="n">
+        <v>0.2240308417219961</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1749,6 +1819,9 @@
       </c>
       <c r="P29" t="n">
         <v>0.4659090909090908</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.7174983936603128</v>
       </c>
     </row>
     <row r="30">
@@ -1796,6 +1869,7 @@
       <c r="P30" t="n">
         <v>0.02651515151515149</v>
       </c>
+      <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1840,6 +1914,7 @@
       <c r="P31" t="n">
         <v>0.8068181818181818</v>
       </c>
+      <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1884,6 +1959,7 @@
       <c r="P32" t="n">
         <v>0</v>
       </c>
+      <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1932,6 +2008,7 @@
       <c r="P33" t="n">
         <v>0.6931818181818181</v>
       </c>
+      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1982,6 +2059,9 @@
       <c r="P34" t="n">
         <v>0.08333333333333331</v>
       </c>
+      <c r="Q34" t="n">
+        <v>0.0610409081173699</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2033,6 +2113,9 @@
       </c>
       <c r="P35" t="n">
         <v>0.7840909090909089</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.7380595416577425</v>
       </c>
     </row>
     <row r="36">
@@ -2060,6 +2143,7 @@
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2112,6 +2196,9 @@
       <c r="P37" t="n">
         <v>0.8371212121212123</v>
       </c>
+      <c r="Q37" t="n">
+        <v>0.8471988495548144</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2164,6 +2251,9 @@
       <c r="P38" t="n">
         <v>0.678030303030303</v>
       </c>
+      <c r="Q38" t="n">
+        <v>0.7402013279074751</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2215,6 +2305,9 @@
       </c>
       <c r="P39" t="n">
         <v>0.5946969696969696</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.6402105069914023</v>
       </c>
     </row>
     <row r="40">
@@ -2262,6 +2355,9 @@
       <c r="P40" t="n">
         <v>0.5946969696969696</v>
       </c>
+      <c r="Q40" t="n">
+        <v>0.2932105375883487</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2311,6 +2407,9 @@
       </c>
       <c r="P41" t="n">
         <v>0.2159090909090909</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.1248967353058165</v>
       </c>
     </row>
     <row r="42">
@@ -2354,6 +2453,9 @@
       <c r="P42" t="n">
         <v>0.3162878787878788</v>
       </c>
+      <c r="Q42" t="n">
+        <v>0.1542698038735734</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2396,6 +2498,9 @@
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2447,6 +2552,9 @@
       </c>
       <c r="P44" t="n">
         <v>0.5757575757575756</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0.5304898571122602</v>
       </c>
     </row>
     <row r="45">
@@ -2492,6 +2600,7 @@
       <c r="P45" t="n">
         <v>0.5189393939393938</v>
       </c>
+      <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2538,6 +2647,7 @@
       <c r="P46" t="n">
         <v>0.4583333333333334</v>
       </c>
+      <c r="Q46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2589,6 +2699,9 @@
       </c>
       <c r="P47" t="n">
         <v>0.6212121212121212</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.5688584279288926</v>
       </c>
     </row>
     <row r="48">
@@ -2616,6 +2729,7 @@
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2650,6 +2764,7 @@
       <c r="P49" t="n">
         <v>0.5795454545454545</v>
       </c>
+      <c r="Q49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2702,6 +2817,7 @@
       <c r="P50" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2752,6 +2868,9 @@
       <c r="P51" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q51" t="n">
+        <v>0.8633540372670806</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2803,6 +2922,9 @@
       </c>
       <c r="P52" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0.9586329284337423</v>
       </c>
     </row>
     <row r="53">
@@ -2852,6 +2974,7 @@
       <c r="P53" t="n">
         <v>0.1439393939393938</v>
       </c>
+      <c r="Q53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2898,6 +3021,7 @@
       <c r="P54" t="n">
         <v>0.2386363636363635</v>
       </c>
+      <c r="Q54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2950,6 +3074,9 @@
       <c r="P55" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3002,6 +3129,9 @@
       <c r="P56" t="n">
         <v>0.4962121212121213</v>
       </c>
+      <c r="Q56" t="n">
+        <v>0.3260716580485268</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3053,6 +3183,9 @@
       </c>
       <c r="P57" t="n">
         <v>0.2878787878787878</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0.1883242052443166</v>
       </c>
     </row>
     <row r="58">
@@ -3080,6 +3213,7 @@
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3106,6 +3240,7 @@
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3132,6 +3267,7 @@
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3158,6 +3294,7 @@
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3184,6 +3321,7 @@
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3230,6 +3368,9 @@
       <c r="P63" t="n">
         <v>0.4583333333333334</v>
       </c>
+      <c r="Q63" t="n">
+        <v>0.4373527521953309</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3279,6 +3420,9 @@
       </c>
       <c r="P64" t="n">
         <v>0.3409090909090909</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0.4757213230119634</v>
       </c>
     </row>
     <row r="65">
@@ -3306,6 +3450,7 @@
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3344,6 +3489,9 @@
       <c r="P66" t="n">
         <v>0.4962121212121213</v>
       </c>
+      <c r="Q66" t="n">
+        <v>0.05054615549368173</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3394,6 +3542,9 @@
       <c r="P67" t="n">
         <v>0.7954545454545455</v>
       </c>
+      <c r="Q67" t="n">
+        <v>0.928464339258942</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3442,6 +3593,7 @@
       <c r="P68" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3485,6 +3637,9 @@
       </c>
       <c r="P69" t="n">
         <v>0.2878787878787878</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0.3480096686350702</v>
       </c>
     </row>
     <row r="70">
@@ -3512,6 +3667,7 @@
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3562,6 +3718,9 @@
       <c r="P71" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q71" t="n">
+        <v>0.9010494752623688</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3612,6 +3771,7 @@
       <c r="P72" t="n">
         <v>0.4204545454545455</v>
       </c>
+      <c r="Q72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3663,6 +3823,9 @@
       </c>
       <c r="P73" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.9832940672520881</v>
       </c>
     </row>
     <row r="74">
@@ -3696,6 +3859,7 @@
       <c r="P74" t="n">
         <v>0.6174242424242423</v>
       </c>
+      <c r="Q74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3746,6 +3910,7 @@
       <c r="P75" t="n">
         <v>0.2462121212121212</v>
       </c>
+      <c r="Q75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3798,6 +3963,9 @@
       <c r="P76" t="n">
         <v>0.7840909090909089</v>
       </c>
+      <c r="Q76" t="n">
+        <v>0.8740629685157419</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3849,6 +4017,9 @@
       </c>
       <c r="P77" t="n">
         <v>0.8371212121212123</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>0.5114891533824923</v>
       </c>
     </row>
     <row r="78">
@@ -3900,6 +4071,9 @@
       <c r="P78" t="n">
         <v>0.3939393939393939</v>
       </c>
+      <c r="Q78" t="n">
+        <v>0.3227671878346541</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3948,6 +4122,9 @@
       <c r="P79" t="n">
         <v>0.3257575757575757</v>
       </c>
+      <c r="Q79" t="n">
+        <v>0.07526848820487715</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3998,6 +4175,7 @@
       <c r="P80" t="n">
         <v>0.4204545454545455</v>
       </c>
+      <c r="Q80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4046,6 +4224,7 @@
       <c r="P81" t="n">
         <v>0.1590909090909091</v>
       </c>
+      <c r="Q81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4094,6 +4273,7 @@
       <c r="P82" t="n">
         <v>0.1249999999999999</v>
       </c>
+      <c r="Q82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4145,6 +4325,9 @@
       </c>
       <c r="P83" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>0.8513600342685801</v>
       </c>
     </row>
     <row r="84">
@@ -4190,6 +4373,7 @@
       </c>
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4237,6 +4421,9 @@
       </c>
       <c r="P85" t="n">
         <v>0.6212121212121212</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>0.2243980050790931</v>
       </c>
     </row>
     <row r="86">
@@ -4264,6 +4451,7 @@
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4314,6 +4502,7 @@
       <c r="P87" t="n">
         <v>0.4204545454545455</v>
       </c>
+      <c r="Q87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4340,6 +4529,7 @@
       </c>
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4387,6 +4577,9 @@
       </c>
       <c r="P89" t="n">
         <v>0.5340909090909092</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>0.2278554600250895</v>
       </c>
     </row>
     <row r="90">
@@ -4414,6 +4607,7 @@
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4462,6 +4656,9 @@
       <c r="P91" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q91" t="n">
+        <v>0.6496037695437996</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4510,6 +4707,9 @@
       <c r="P92" t="n">
         <v>0.4583333333333334</v>
       </c>
+      <c r="Q92" t="n">
+        <v>0.02998500749625187</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4561,6 +4761,9 @@
       </c>
       <c r="P93" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q93" t="n">
+        <v>0.8010280573998714</v>
       </c>
     </row>
     <row r="94">
@@ -4588,6 +4791,7 @@
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4614,6 +4818,7 @@
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4640,6 +4845,7 @@
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
       <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4666,6 +4872,7 @@
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4715,6 +4922,9 @@
       </c>
       <c r="P98" t="n">
         <v>0.7083333333333333</v>
+      </c>
+      <c r="Q98" t="n">
+        <v>0.5043906618119512</v>
       </c>
     </row>
     <row r="99">
@@ -4742,6 +4952,7 @@
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr"/>
       <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4792,6 +5003,9 @@
       <c r="P100" t="n">
         <v>0.3787878787878788</v>
       </c>
+      <c r="Q100" t="n">
+        <v>0.74863996573142</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4844,6 +5058,9 @@
       <c r="P101" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q101" t="n">
+        <v>0.9434568430070679</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4896,6 +5113,7 @@
       <c r="P102" t="n">
         <v>0.2575757575757575</v>
       </c>
+      <c r="Q102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4942,6 +5160,7 @@
       </c>
       <c r="O103" t="inlineStr"/>
       <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4994,6 +5213,7 @@
       <c r="P104" t="n">
         <v>0.731060606060606</v>
       </c>
+      <c r="Q104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5046,6 +5266,9 @@
       <c r="P105" t="n">
         <v>0.7727272727272727</v>
       </c>
+      <c r="Q105" t="n">
+        <v>0.3801058654346297</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5097,6 +5320,9 @@
       </c>
       <c r="P106" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>0.9374598415078176</v>
       </c>
     </row>
     <row r="107">
@@ -5146,6 +5372,9 @@
       <c r="P107" t="n">
         <v>0.5568181818181817</v>
       </c>
+      <c r="Q107" t="n">
+        <v>0.3456843007067894</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5190,6 +5419,9 @@
       <c r="P108" t="n">
         <v>0.5530303030303031</v>
       </c>
+      <c r="Q108" t="n">
+        <v>0.4020438760211731</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5241,6 +5473,9 @@
       </c>
       <c r="P109" t="n">
         <v>0.6363636363636362</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>0.6995073891625616</v>
       </c>
     </row>
     <row r="110">
@@ -5292,6 +5527,9 @@
       <c r="P110" t="n">
         <v>0.6136363636363635</v>
       </c>
+      <c r="Q110" t="n">
+        <v>0.2529143591469571</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5340,6 +5578,9 @@
       <c r="P111" t="n">
         <v>0.2840909090909091</v>
       </c>
+      <c r="Q111" t="n">
+        <v>0.4611265795673592</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5388,6 +5629,9 @@
       <c r="P112" t="n">
         <v>0.5606060606060606</v>
       </c>
+      <c r="Q112" t="n">
+        <v>0.1620720252118839</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5435,6 +5679,9 @@
       </c>
       <c r="P113" t="n">
         <v>0.5416666666666666</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>0.1555854725698376</v>
       </c>
     </row>
     <row r="114">
@@ -5478,6 +5725,7 @@
       <c r="P114" t="n">
         <v>0.7159090909090909</v>
       </c>
+      <c r="Q114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5508,6 +5756,7 @@
       </c>
       <c r="O115" t="inlineStr"/>
       <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5553,6 +5802,9 @@
       </c>
       <c r="P116" t="n">
         <v>0.5909090909090909</v>
+      </c>
+      <c r="Q116" t="n">
+        <v>0.6729492396658814</v>
       </c>
     </row>
     <row r="117">
@@ -5580,6 +5832,7 @@
       <c r="N117" t="inlineStr"/>
       <c r="O117" t="inlineStr"/>
       <c r="P117" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5627,6 +5880,9 @@
       </c>
       <c r="P118" t="n">
         <v>0.6325757575757575</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>0.100663953737417</v>
       </c>
     </row>
     <row r="119">
@@ -5654,6 +5910,7 @@
       <c r="N119" t="inlineStr"/>
       <c r="O119" t="inlineStr"/>
       <c r="P119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5701,6 +5958,9 @@
       </c>
       <c r="P120" t="n">
         <v>0.4810606060606059</v>
+      </c>
+      <c r="Q120" t="n">
+        <v>0.2410121469877306</v>
       </c>
     </row>
     <row r="121">
@@ -5744,6 +6004,9 @@
       <c r="P121" t="n">
         <v>0.5530303030303031</v>
       </c>
+      <c r="Q121" t="n">
+        <v>0.3507327968668726</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5789,6 +6052,9 @@
       </c>
       <c r="P122" t="n">
         <v>0.4659090909090908</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>0.1319952268763578</v>
       </c>
     </row>
     <row r="123">
@@ -5830,6 +6096,7 @@
         <v>0.8761384335154827</v>
       </c>
       <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5876,6 +6143,7 @@
       <c r="P124" t="n">
         <v>0.3371212121212121</v>
       </c>
+      <c r="Q124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5902,6 +6170,7 @@
       <c r="N125" t="inlineStr"/>
       <c r="O125" t="inlineStr"/>
       <c r="P125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5928,6 +6197,7 @@
       <c r="N126" t="inlineStr"/>
       <c r="O126" t="inlineStr"/>
       <c r="P126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5954,6 +6224,7 @@
       <c r="P127" t="n">
         <v>0.8371212121212123</v>
       </c>
+      <c r="Q127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -6003,6 +6274,9 @@
       </c>
       <c r="P128" t="n">
         <v>0.5113636363636364</v>
+      </c>
+      <c r="Q128" t="n">
+        <v>0.4398922987485849</v>
       </c>
     </row>
     <row r="129">
@@ -6030,6 +6304,7 @@
       <c r="N129" t="inlineStr"/>
       <c r="O129" t="inlineStr"/>
       <c r="P129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6056,6 +6331,7 @@
       <c r="N130" t="inlineStr"/>
       <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -6104,6 +6380,7 @@
       <c r="P131" t="n">
         <v>0.3598484848484849</v>
       </c>
+      <c r="Q131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -6130,6 +6407,7 @@
       <c r="N132" t="inlineStr"/>
       <c r="O132" t="inlineStr"/>
       <c r="P132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -6180,6 +6458,7 @@
       <c r="P133" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -6232,6 +6511,7 @@
       <c r="P134" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -6282,6 +6562,7 @@
       <c r="P135" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6332,6 +6613,9 @@
       <c r="P136" t="n">
         <v>0.4772727272727273</v>
       </c>
+      <c r="Q136" t="n">
+        <v>0.440840804087752</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -6383,6 +6667,9 @@
       </c>
       <c r="P137" t="n">
         <v>0.6401515151515151</v>
+      </c>
+      <c r="Q137" t="n">
+        <v>0.2508643637364991</v>
       </c>
     </row>
     <row r="138">
@@ -6429,6 +6716,9 @@
       </c>
       <c r="P138" t="n">
         <v>0.4962121212121213</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>0.07416699813358628</v>
       </c>
     </row>
     <row r="139">
@@ -6465,6 +6755,9 @@
       </c>
       <c r="P139" t="n">
         <v>0.3863636363636364</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0.174983936603127</v>
       </c>
     </row>
     <row r="140">
@@ -6492,6 +6785,7 @@
       <c r="N140" t="inlineStr"/>
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="inlineStr"/>
+      <c r="Q140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6543,6 +6837,9 @@
       </c>
       <c r="P141" t="n">
         <v>0.6553030303030303</v>
+      </c>
+      <c r="Q141" t="n">
+        <v>0.8316556007710431</v>
       </c>
     </row>
     <row r="142">
@@ -6572,6 +6869,7 @@
       </c>
       <c r="O142" t="inlineStr"/>
       <c r="P142" t="inlineStr"/>
+      <c r="Q142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6623,6 +6921,9 @@
       </c>
       <c r="P143" t="n">
         <v>0.6742424242424242</v>
+      </c>
+      <c r="Q143" t="n">
+        <v>0.4201572683046232</v>
       </c>
     </row>
     <row r="144">
@@ -6672,6 +6973,9 @@
       <c r="P144" t="n">
         <v>0.4128787878787878</v>
       </c>
+      <c r="Q144" t="n">
+        <v>0.2498852614509072</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6722,6 +7026,7 @@
       <c r="P145" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6767,6 +7072,9 @@
       </c>
       <c r="P146" t="n">
         <v>0.5189393939393938</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>0.1377168558577854</v>
       </c>
     </row>
     <row r="147">
@@ -6794,6 +7102,7 @@
       <c r="N147" t="inlineStr"/>
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6842,6 +7151,9 @@
       <c r="P148" t="n">
         <v>0.6931818181818181</v>
       </c>
+      <c r="Q148" t="n">
+        <v>0.4595355383532724</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6892,6 +7204,9 @@
       <c r="P149" t="n">
         <v>0.609848484848485</v>
       </c>
+      <c r="Q149" t="n">
+        <v>0.07774684086528166</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6938,6 +7253,9 @@
       <c r="P150" t="n">
         <v>0.5378787878787877</v>
       </c>
+      <c r="Q150" t="n">
+        <v>0.3521096594559864</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6985,6 +7303,9 @@
       </c>
       <c r="P151" t="n">
         <v>0.3939393939393939</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>0.1307101551265184</v>
       </c>
     </row>
     <row r="152">
@@ -7012,6 +7333,7 @@
       <c r="N152" t="inlineStr"/>
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="inlineStr"/>
+      <c r="Q152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -7060,6 +7382,7 @@
       <c r="P153" t="n">
         <v>0.8560606060606062</v>
       </c>
+      <c r="Q153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -7108,6 +7431,9 @@
       <c r="P154" t="n">
         <v>0.4962121212121213</v>
       </c>
+      <c r="Q154" t="n">
+        <v>0.4045834225744271</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -7159,6 +7485,9 @@
       </c>
       <c r="P155" t="n">
         <v>0.7727272727272727</v>
+      </c>
+      <c r="Q155" t="n">
+        <v>0.287978459749717</v>
       </c>
     </row>
     <row r="156">
@@ -7186,6 +7515,7 @@
       <c r="N156" t="inlineStr"/>
       <c r="O156" t="inlineStr"/>
       <c r="P156" t="inlineStr"/>
+      <c r="Q156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -7234,6 +7564,7 @@
       <c r="P157" t="n">
         <v>0.5643939393939393</v>
       </c>
+      <c r="Q157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -7280,6 +7611,9 @@
       <c r="P158" t="n">
         <v>0.3939393939393939</v>
       </c>
+      <c r="Q158" t="n">
+        <v>0.1546369672306704</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -7331,6 +7665,9 @@
       </c>
       <c r="P159" t="n">
         <v>0.4810606060606059</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>0.33956491142184</v>
       </c>
     </row>
     <row r="160">
@@ -7382,6 +7719,9 @@
       <c r="P160" t="n">
         <v>0.4772727272727273</v>
       </c>
+      <c r="Q160" t="n">
+        <v>0.379585717345409</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -7434,6 +7774,9 @@
       <c r="P161" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q161" t="n">
+        <v>0.9201113728849861</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -7485,6 +7828,9 @@
       </c>
       <c r="P162" t="n">
         <v>0.8068181818181818</v>
+      </c>
+      <c r="Q162" t="n">
+        <v>0.7682587277789678</v>
       </c>
     </row>
     <row r="163">
@@ -7529,6 +7875,9 @@
       </c>
       <c r="P163" t="n">
         <v>0.303030303030303</v>
+      </c>
+      <c r="Q163" t="n">
+        <v>0.1997368662607472</v>
       </c>
     </row>
     <row r="164">
@@ -7562,6 +7911,7 @@
       </c>
       <c r="O164" t="inlineStr"/>
       <c r="P164" t="inlineStr"/>
+      <c r="Q164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -7613,6 +7963,9 @@
       </c>
       <c r="P165" t="n">
         <v>0.9015151515151515</v>
+      </c>
+      <c r="Q165" t="n">
+        <v>0.6498179481687727</v>
       </c>
     </row>
     <row r="166">
@@ -7661,6 +8014,9 @@
       </c>
       <c r="P166" t="n">
         <v>0.6439393939393939</v>
+      </c>
+      <c r="Q166" t="n">
+        <v>0.3735275219533091</v>
       </c>
     </row>
     <row r="167">
@@ -7686,6 +8042,7 @@
       <c r="N167" t="inlineStr"/>
       <c r="O167" t="inlineStr"/>
       <c r="P167" t="inlineStr"/>
+      <c r="Q167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -7710,6 +8067,7 @@
       <c r="N168" t="inlineStr"/>
       <c r="O168" t="inlineStr"/>
       <c r="P168" t="inlineStr"/>
+      <c r="Q168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -7760,6 +8118,9 @@
       <c r="P169" t="n">
         <v>0.4810606060606059</v>
       </c>
+      <c r="Q169" t="n">
+        <v>0.2310375424532631</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -7808,6 +8169,9 @@
       <c r="P170" t="n">
         <v>0.6856060606060607</v>
       </c>
+      <c r="Q170" t="n">
+        <v>0.3037052902120368</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -7858,6 +8222,9 @@
       <c r="P171" t="n">
         <v>0.7424242424242425</v>
       </c>
+      <c r="Q171" t="n">
+        <v>0.2664076125202705</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -7909,6 +8276,9 @@
       </c>
       <c r="P172" t="n">
         <v>0.609848484848485</v>
+      </c>
+      <c r="Q172" t="n">
+        <v>0.4196677171618273</v>
       </c>
     </row>
     <row r="173">
@@ -7960,6 +8330,9 @@
       <c r="P173" t="n">
         <v>0.6742424242424242</v>
       </c>
+      <c r="Q173" t="n">
+        <v>0.2490285469510143</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8011,6 +8384,9 @@
       </c>
       <c r="P174" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q174" t="n">
+        <v>0.6919805403420739</v>
       </c>
     </row>
     <row r="175">
@@ -8038,6 +8414,7 @@
       <c r="N175" t="inlineStr"/>
       <c r="O175" t="inlineStr"/>
       <c r="P175" t="inlineStr"/>
+      <c r="Q175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8062,6 +8439,7 @@
       <c r="N176" t="inlineStr"/>
       <c r="O176" t="inlineStr"/>
       <c r="P176" t="inlineStr"/>
+      <c r="Q176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -8113,6 +8491,9 @@
       </c>
       <c r="P177" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q177" t="n">
+        <v>0.8822017562647249</v>
       </c>
     </row>
     <row r="178">
@@ -8163,6 +8544,9 @@
       </c>
       <c r="P178" t="n">
         <v>0.662878787878788</v>
+      </c>
+      <c r="Q178" t="n">
+        <v>0.3212373405134167</v>
       </c>
     </row>
     <row r="179">
@@ -8194,6 +8578,9 @@
       </c>
       <c r="O179" t="inlineStr"/>
       <c r="P179" t="inlineStr"/>
+      <c r="Q179" t="n">
+        <v>0.1158706361105162</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -8218,6 +8605,7 @@
       <c r="N180" t="inlineStr"/>
       <c r="O180" t="inlineStr"/>
       <c r="P180" t="inlineStr"/>
+      <c r="Q180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -8244,6 +8632,7 @@
       <c r="N181" t="inlineStr"/>
       <c r="O181" t="inlineStr"/>
       <c r="P181" t="inlineStr"/>
+      <c r="Q181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -8293,6 +8682,9 @@
       </c>
       <c r="P182" t="n">
         <v>0.7462121212121211</v>
+      </c>
+      <c r="Q182" t="n">
+        <v>0.2459382553621148</v>
       </c>
     </row>
     <row r="183">
@@ -8320,6 +8712,7 @@
       <c r="N183" t="inlineStr"/>
       <c r="O183" t="inlineStr"/>
       <c r="P183" t="inlineStr"/>
+      <c r="Q183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -8346,6 +8739,7 @@
       <c r="N184" t="inlineStr"/>
       <c r="O184" t="inlineStr"/>
       <c r="P184" t="inlineStr"/>
+      <c r="Q184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -8394,6 +8788,9 @@
       <c r="P185" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q185" t="n">
+        <v>0.7254230027843223</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -8444,6 +8841,9 @@
       <c r="P186" t="n">
         <v>0.5151515151515152</v>
       </c>
+      <c r="Q186" t="n">
+        <v>0.3069179695866353</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -8491,6 +8891,9 @@
       </c>
       <c r="P187" t="n">
         <v>0.2196969696969696</v>
+      </c>
+      <c r="Q187" t="n">
+        <v>0.5089802037756632</v>
       </c>
     </row>
     <row r="188">
@@ -8518,6 +8921,7 @@
       <c r="N188" t="inlineStr"/>
       <c r="O188" t="inlineStr"/>
       <c r="P188" t="inlineStr"/>
+      <c r="Q188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -8569,6 +8973,9 @@
       </c>
       <c r="P189" t="n">
         <v>0.6060606060606061</v>
+      </c>
+      <c r="Q189" t="n">
+        <v>0.2325979867209252</v>
       </c>
     </row>
     <row r="190">
@@ -8612,6 +9019,9 @@
         <v>0.726775956284153</v>
       </c>
       <c r="P190" t="inlineStr"/>
+      <c r="Q190" t="n">
+        <v>0.09087293088149803</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -8658,6 +9068,9 @@
       <c r="P191" t="n">
         <v>0.4545454545454546</v>
       </c>
+      <c r="Q191" t="n">
+        <v>0.2842150353394731</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -8709,6 +9122,9 @@
       </c>
       <c r="P192" t="n">
         <v>1</v>
+      </c>
+      <c r="Q192" t="n">
+        <v>0.4856653306000062</v>
       </c>
     </row>
     <row r="193">
@@ -8760,6 +9176,9 @@
       <c r="P193" t="n">
         <v>0.4356060606060606</v>
       </c>
+      <c r="Q193" t="n">
+        <v>0.1032646941835205</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -8808,6 +9227,9 @@
       <c r="P194" t="n">
         <v>0.4053030303030303</v>
       </c>
+      <c r="Q194" t="n">
+        <v>0.1218676376097665</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -8855,6 +9277,9 @@
       </c>
       <c r="P195" t="n">
         <v>0.5265151515151515</v>
+      </c>
+      <c r="Q195" t="n">
+        <v>0.2814613101612459</v>
       </c>
     </row>
     <row r="196">
@@ -8894,6 +9319,9 @@
       </c>
       <c r="O196" t="inlineStr"/>
       <c r="P196" t="inlineStr"/>
+      <c r="Q196" t="n">
+        <v>0.008995502248875561</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -8943,6 +9371,9 @@
       </c>
       <c r="P197" t="n">
         <v>0.6515151515151514</v>
+      </c>
+      <c r="Q197" t="n">
+        <v>0.551173392895389</v>
       </c>
     </row>
     <row r="198">
@@ -8970,6 +9401,7 @@
       <c r="N198" t="inlineStr"/>
       <c r="O198" t="inlineStr"/>
       <c r="P198" t="inlineStr"/>
+      <c r="Q198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -9002,6 +9434,9 @@
       <c r="N199" t="inlineStr"/>
       <c r="O199" t="inlineStr"/>
       <c r="P199" t="inlineStr"/>
+      <c r="Q199" t="n">
+        <v>0.003212679374598414</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -9028,6 +9463,7 @@
       <c r="N200" t="inlineStr"/>
       <c r="O200" t="inlineStr"/>
       <c r="P200" t="inlineStr"/>
+      <c r="Q200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -9074,6 +9510,7 @@
       <c r="P201" t="n">
         <v>0.4318181818181818</v>
       </c>
+      <c r="Q201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -9120,6 +9557,7 @@
       <c r="P202" t="n">
         <v>0.4166666666666667</v>
       </c>
+      <c r="Q202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -9170,6 +9608,9 @@
       <c r="P203" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q203" t="n">
+        <v>0.8160205611479975</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -9218,6 +9659,7 @@
       <c r="P204" t="n">
         <v>0.7007575757575758</v>
       </c>
+      <c r="Q204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -9269,6 +9711,9 @@
       </c>
       <c r="P205" t="n">
         <v>0.7007575757575758</v>
+      </c>
+      <c r="Q205" t="n">
+        <v>0.9264449407949086</v>
       </c>
     </row>
     <row r="206">
@@ -9314,6 +9759,7 @@
       <c r="P206" t="n">
         <v>0.5946969696969696</v>
       </c>
+      <c r="Q206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -9348,6 +9794,7 @@
       <c r="P207" t="n">
         <v>0.7196969696969697</v>
       </c>
+      <c r="Q207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -9382,6 +9829,7 @@
       </c>
       <c r="O208" t="inlineStr"/>
       <c r="P208" t="inlineStr"/>
+      <c r="Q208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -9427,6 +9875,9 @@
       </c>
       <c r="P209" t="n">
         <v>0.0946969696969697</v>
+      </c>
+      <c r="Q209" t="n">
+        <v>0.335832083958021</v>
       </c>
     </row>
     <row r="210">
@@ -9454,6 +9905,7 @@
       <c r="N210" t="inlineStr"/>
       <c r="O210" t="inlineStr"/>
       <c r="P210" t="inlineStr"/>
+      <c r="Q210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -9480,6 +9932,7 @@
       <c r="N211" t="inlineStr"/>
       <c r="O211" t="inlineStr"/>
       <c r="P211" t="inlineStr"/>
+      <c r="Q211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -9530,6 +9983,9 @@
       <c r="P212" t="n">
         <v>0.4318181818181818</v>
       </c>
+      <c r="Q212" t="n">
+        <v>0.3184224214423401</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -9580,6 +10036,9 @@
       <c r="P213" t="n">
         <v>0.5795454545454545</v>
       </c>
+      <c r="Q213" t="n">
+        <v>0.5382308845577212</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -9628,6 +10087,9 @@
       <c r="P214" t="n">
         <v>0.5681818181818182</v>
       </c>
+      <c r="Q214" t="n">
+        <v>0.1550959214270416</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -9671,6 +10133,9 @@
       </c>
       <c r="P215" t="n">
         <v>0.6060606060606061</v>
+      </c>
+      <c r="Q215" t="n">
+        <v>0.001070893124866138</v>
       </c>
     </row>
     <row r="216">
@@ -9698,6 +10163,7 @@
       <c r="N216" t="inlineStr"/>
       <c r="O216" t="inlineStr"/>
       <c r="P216" t="inlineStr"/>
+      <c r="Q216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -9728,6 +10194,7 @@
       <c r="N217" t="inlineStr"/>
       <c r="O217" t="inlineStr"/>
       <c r="P217" t="inlineStr"/>
+      <c r="Q217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -9754,6 +10221,7 @@
       <c r="N218" t="inlineStr"/>
       <c r="O218" t="inlineStr"/>
       <c r="P218" t="inlineStr"/>
+      <c r="Q218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -9780,6 +10248,7 @@
       <c r="N219" t="inlineStr"/>
       <c r="O219" t="inlineStr"/>
       <c r="P219" t="inlineStr"/>
+      <c r="Q219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -9812,6 +10281,7 @@
       <c r="P220" t="n">
         <v>0.5606060606060606</v>
       </c>
+      <c r="Q220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -9838,6 +10308,7 @@
       <c r="N221" t="inlineStr"/>
       <c r="O221" t="inlineStr"/>
       <c r="P221" t="inlineStr"/>
+      <c r="Q221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -9864,6 +10335,7 @@
       <c r="N222" t="inlineStr"/>
       <c r="O222" t="inlineStr"/>
       <c r="P222" t="inlineStr"/>
+      <c r="Q222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -9916,6 +10388,7 @@
       <c r="P223" t="n">
         <v>0.4999999999999999</v>
       </c>
+      <c r="Q223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -9966,6 +10439,9 @@
       <c r="P224" t="n">
         <v>0.2083333333333333</v>
       </c>
+      <c r="Q224" t="n">
+        <v>0.4686840253342716</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -10015,6 +10491,9 @@
       </c>
       <c r="P225" t="n">
         <v>0.5416666666666666</v>
+      </c>
+      <c r="Q225" t="n">
+        <v>0.6000367163357097</v>
       </c>
     </row>
     <row r="226">
@@ -10042,6 +10521,7 @@
       </c>
       <c r="O226" t="inlineStr"/>
       <c r="P226" t="inlineStr"/>
+      <c r="Q226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -10082,6 +10562,7 @@
       <c r="P227" t="n">
         <v>0.8371212121212123</v>
       </c>
+      <c r="Q227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -10128,6 +10609,9 @@
       <c r="P228" t="n">
         <v>0.3484848484848485</v>
       </c>
+      <c r="Q228" t="n">
+        <v>0.2248569592754643</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -10176,6 +10660,9 @@
       <c r="P229" t="n">
         <v>0.2575757575757575</v>
       </c>
+      <c r="Q229" t="n">
+        <v>0.2783710185723465</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -10225,6 +10712,9 @@
       <c r="O230" t="inlineStr"/>
       <c r="P230" t="n">
         <v>0.5871212121212122</v>
+      </c>
+      <c r="Q230" t="n">
+        <v>0.5694397699109628</v>
       </c>
     </row>
     <row r="231">
@@ -10252,6 +10742,7 @@
       <c r="N231" t="inlineStr"/>
       <c r="O231" t="inlineStr"/>
       <c r="P231" t="inlineStr"/>
+      <c r="Q231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -10304,6 +10795,9 @@
       <c r="P232" t="n">
         <v>0.5492424242424243</v>
       </c>
+      <c r="Q232" t="n">
+        <v>0.5870636110516171</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -10355,6 +10849,9 @@
       </c>
       <c r="P233" t="n">
         <v>0.6325757575757575</v>
+      </c>
+      <c r="Q233" t="n">
+        <v>0.8522167487684729</v>
       </c>
     </row>
     <row r="234">
@@ -10405,6 +10902,9 @@
       </c>
       <c r="P234" t="n">
         <v>0.6325757575757575</v>
+      </c>
+      <c r="Q234" t="n">
+        <v>0.1521280176238411</v>
       </c>
     </row>
     <row r="235">
@@ -10452,6 +10952,7 @@
       <c r="P235" t="n">
         <v>0.2954545454545454</v>
       </c>
+      <c r="Q235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -10494,6 +10995,9 @@
       <c r="P236" t="n">
         <v>0</v>
       </c>
+      <c r="Q236" t="n">
+        <v>0.08766025150689963</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -10543,6 +11047,9 @@
       </c>
       <c r="P237" t="n">
         <v>0.712121212121212</v>
+      </c>
+      <c r="Q237" t="n">
+        <v>0.4255729278218035</v>
       </c>
     </row>
     <row r="238">
@@ -10587,6 +11094,9 @@
       </c>
       <c r="P238" t="n">
         <v>0.3295454545454545</v>
+      </c>
+      <c r="Q238" t="n">
+        <v>0.0610409081173699</v>
       </c>
     </row>
     <row r="239">
@@ -10614,6 +11124,7 @@
       <c r="N239" t="inlineStr"/>
       <c r="O239" t="inlineStr"/>
       <c r="P239" t="inlineStr"/>
+      <c r="Q239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -10660,6 +11171,7 @@
       <c r="P240" t="n">
         <v>0.4734848484848485</v>
       </c>
+      <c r="Q240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -10688,6 +11200,9 @@
       <c r="N241" t="inlineStr"/>
       <c r="O241" t="inlineStr"/>
       <c r="P241" t="inlineStr"/>
+      <c r="Q241" t="n">
+        <v>0.3838998867912983</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -10720,6 +11235,9 @@
       <c r="N242" t="inlineStr"/>
       <c r="O242" t="inlineStr"/>
       <c r="P242" t="inlineStr"/>
+      <c r="Q242" t="n">
+        <v>0.1606339687299208</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -10771,6 +11289,9 @@
       </c>
       <c r="P243" t="n">
         <v>0.571969696969697</v>
+      </c>
+      <c r="Q243" t="n">
+        <v>0.5894195759263225</v>
       </c>
     </row>
     <row r="244">
@@ -10798,6 +11319,7 @@
       <c r="N244" t="inlineStr"/>
       <c r="O244" t="inlineStr"/>
       <c r="P244" t="inlineStr"/>
+      <c r="Q244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -10845,6 +11367,9 @@
       </c>
       <c r="P245" t="n">
         <v>0.4015151515151514</v>
+      </c>
+      <c r="Q245" t="n">
+        <v>0.2235412905792002</v>
       </c>
     </row>
     <row r="246">
@@ -10890,6 +11415,9 @@
       <c r="P246" t="n">
         <v>0.1553030303030302</v>
       </c>
+      <c r="Q246" t="n">
+        <v>0.3441238564391274</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>